<commit_message>
Change fornt to [Carlito] in example 15
</commit_message>
<xml_diff>
--- a/ampl-data-input-excel/15-public-holidays/15-public-holidays.xlsx
+++ b/ampl-data-input-excel/15-public-holidays/15-public-holidays.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="14"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="experts" sheetId="1" state="visible" r:id="rId3"/>
@@ -406,10 +406,10 @@
     <numFmt numFmtId="166" formatCode="@"/>
     <numFmt numFmtId="167" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="9">
     <font>
       <sz val="10"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
@@ -430,6 +430,12 @@
     </font>
     <font>
       <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -442,22 +448,12 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <b val="true"/>
       <sz val="10"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <b val="true"/>
@@ -550,43 +546,99 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -594,79 +646,23 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -853,18 +849,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D1048576"/>
+  <dimension ref="A1:D1004"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.71484375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="18.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="15.2"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="11.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="3" width="12.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="20.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="16.7"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="12.71"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="4" style="3" width="12.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="13.35"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="6" style="3" width="12.71"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3933,19 +3931,6 @@
     <row r="1004" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C1004" s="6"/>
     </row>
-    <row r="1048564" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048565" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048566" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048567" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -3969,41 +3954,42 @@
       <selection pane="topLeft" activeCell="G11" activeCellId="0" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.71484375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="19.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="24" width="13.71"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="3" style="7" width="11.57"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="5" style="6" width="11.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="21.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="23" width="15.07"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="3" style="7" width="12.71"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="5" style="6" width="12.71"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="7" style="3" width="12.71"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="E1" s="5" t="b">
+      <c r="E1" s="16" t="b">
         <f aca="false">AND(E2:E832)</f>
         <v>1</v>
       </c>
-      <c r="F1" s="5" t="b">
+      <c r="F1" s="16" t="b">
         <f aca="false">AND(F2:F832)</f>
         <v>1</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="20" t="s">
         <v>16</v>
       </c>
       <c r="C2" s="1" t="n">
@@ -4023,10 +4009,10 @@
       <c r="G2" s="1"/>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="21" t="s">
+      <c r="B3" s="20" t="s">
         <v>17</v>
       </c>
       <c r="C3" s="1" t="n">
@@ -4049,7 +4035,7 @@
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="21" t="s">
+      <c r="B4" s="20" t="s">
         <v>16</v>
       </c>
       <c r="C4" s="1" t="n">
@@ -4072,7 +4058,7 @@
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="21" t="s">
+      <c r="B5" s="20" t="s">
         <v>17</v>
       </c>
       <c r="C5" s="1" t="n">
@@ -4095,7 +4081,7 @@
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="21" t="s">
+      <c r="B6" s="20" t="s">
         <v>16</v>
       </c>
       <c r="C6" s="1" t="n">
@@ -4118,7 +4104,7 @@
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="21" t="s">
+      <c r="B7" s="20" t="s">
         <v>17</v>
       </c>
       <c r="C7" s="1" t="n">
@@ -4138,43 +4124,37 @@
       <c r="G7" s="1"/>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="16"/>
-      <c r="B8" s="23"/>
+      <c r="B8" s="22"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="G8" s="1"/>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="16"/>
-      <c r="B9" s="23"/>
+      <c r="B9" s="22"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="G9" s="1"/>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="16"/>
-      <c r="B10" s="23"/>
+      <c r="B10" s="22"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="G10" s="1"/>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="16"/>
-      <c r="B11" s="23"/>
+      <c r="B11" s="22"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="G11" s="1"/>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="16"/>
-      <c r="B12" s="23"/>
+      <c r="B12" s="22"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="G12" s="1"/>
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="16"/>
-      <c r="B13" s="23"/>
+      <c r="B13" s="22"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="G13" s="1"/>
@@ -4202,24 +4182,25 @@
       <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.71484375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="7" width="11.57"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="6" width="11.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="25" width="16.05"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="7" width="12.71"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="6" width="12.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="7" width="17.64"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="4" style="3" width="12.71"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="11" t="b">
+      <c r="B1" s="25" t="b">
         <f aca="false">AND(B2:B905)</f>
         <v>1</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="14" t="n">
+      <c r="A2" s="13" t="n">
         <v>45658</v>
       </c>
       <c r="B2" s="6" t="b">
@@ -4228,7 +4209,7 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="14" t="n">
+      <c r="A3" s="13" t="n">
         <v>45661</v>
       </c>
       <c r="B3" s="6" t="b">
@@ -4240,133 +4221,133 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="14"/>
+      <c r="A4" s="13"/>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="14"/>
+      <c r="A5" s="13"/>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="14"/>
+      <c r="A6" s="13"/>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="14"/>
+      <c r="A7" s="13"/>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="14"/>
+      <c r="A8" s="13"/>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="14"/>
+      <c r="A9" s="13"/>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="14"/>
+      <c r="A10" s="13"/>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="14"/>
+      <c r="A11" s="13"/>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="14"/>
+      <c r="A12" s="13"/>
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="14"/>
+      <c r="A13" s="13"/>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="14"/>
+      <c r="A14" s="13"/>
     </row>
     <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="14"/>
+      <c r="A15" s="13"/>
     </row>
     <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="14"/>
+      <c r="A16" s="13"/>
     </row>
     <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="14"/>
+      <c r="A17" s="13"/>
     </row>
     <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="14"/>
+      <c r="A18" s="13"/>
     </row>
     <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="14"/>
+      <c r="A19" s="13"/>
     </row>
     <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="14"/>
+      <c r="A20" s="13"/>
     </row>
     <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="14"/>
+      <c r="A21" s="13"/>
     </row>
     <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="14"/>
+      <c r="A22" s="13"/>
     </row>
     <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="14"/>
+      <c r="A23" s="13"/>
     </row>
     <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="14"/>
+      <c r="A24" s="13"/>
     </row>
     <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="14"/>
+      <c r="A25" s="13"/>
     </row>
     <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="14"/>
+      <c r="A26" s="13"/>
     </row>
     <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="14"/>
+      <c r="A27" s="13"/>
     </row>
     <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="14"/>
+      <c r="A28" s="13"/>
     </row>
     <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="14"/>
+      <c r="A29" s="13"/>
     </row>
     <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="14"/>
+      <c r="A30" s="13"/>
     </row>
     <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="14"/>
+      <c r="A31" s="13"/>
     </row>
     <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="14"/>
+      <c r="A32" s="13"/>
     </row>
     <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="14"/>
+      <c r="A33" s="13"/>
     </row>
     <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="14"/>
+      <c r="A34" s="13"/>
     </row>
     <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="14"/>
+      <c r="A35" s="13"/>
     </row>
     <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="14"/>
+      <c r="A36" s="13"/>
     </row>
     <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="14"/>
+      <c r="A37" s="13"/>
     </row>
     <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="14"/>
+      <c r="A38" s="13"/>
     </row>
     <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="14"/>
+      <c r="A39" s="13"/>
     </row>
     <row r="40" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="14"/>
+      <c r="A40" s="13"/>
     </row>
     <row r="41" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="14"/>
+      <c r="A41" s="13"/>
     </row>
     <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="14"/>
+      <c r="A42" s="13"/>
     </row>
     <row r="43" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="14"/>
+      <c r="A43" s="13"/>
     </row>
     <row r="44" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="14"/>
+      <c r="A44" s="13"/>
     </row>
     <row r="45" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="14"/>
+      <c r="A45" s="13"/>
     </row>
     <row r="46" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="14"/>
+      <c r="A46" s="13"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -4388,24 +4369,25 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="F22" activeCellId="0" sqref="F22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.71484375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="7" width="11.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="7" width="19.42"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="11.57"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="7" width="12.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="7" width="21.35"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="12.71"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="4" style="3" width="12.71"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="24" t="s">
         <v>23</v>
       </c>
       <c r="D1" s="27" t="s">
@@ -4413,7 +4395,7 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="14" t="n">
+      <c r="A2" s="13" t="n">
         <v>45655</v>
       </c>
       <c r="B2" s="7" t="n">
@@ -4446,42 +4428,43 @@
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
+      <selection pane="topLeft" activeCell="K35" activeCellId="0" sqref="K35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.67578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="24.46"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="12" min="2" style="1" width="11.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="3" width="23.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="26.88"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="12" min="2" style="1" width="12.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="25.47"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="14" style="3" width="12.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="G1" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="H1" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="I1" s="10" t="s">
+      <c r="I1" s="24" t="s">
         <v>31</v>
       </c>
       <c r="J1" s="27" t="s">
@@ -4501,17 +4484,17 @@
       <c r="D2" s="7" t="n">
         <v>150</v>
       </c>
-      <c r="E2" s="14" t="n">
+      <c r="E2" s="13" t="n">
         <f aca="false">misc!A2+1</f>
         <v>45656</v>
       </c>
       <c r="F2" s="12" t="n">
         <v>45671</v>
       </c>
-      <c r="G2" s="14" t="s">
+      <c r="G2" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="H2" s="14" t="s">
+      <c r="H2" s="13" t="s">
         <v>35</v>
       </c>
       <c r="I2" s="7" t="n">
@@ -4548,38 +4531,39 @@
       <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.67578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="24.46"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="9" min="2" style="1" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="26.88"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="9" min="2" style="1" width="12.67"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="10" style="3" width="12.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="G1" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="H1" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="I1" s="10" t="s">
+      <c r="I1" s="24" t="s">
         <v>31</v>
       </c>
       <c r="J1" s="27" t="s">
@@ -4599,17 +4583,17 @@
       <c r="D2" s="7" t="n">
         <v>150</v>
       </c>
-      <c r="E2" s="14" t="n">
+      <c r="E2" s="13" t="n">
         <f aca="false">misc!A2+1</f>
         <v>45656</v>
       </c>
       <c r="F2" s="12" t="n">
         <v>45671</v>
       </c>
-      <c r="G2" s="14" t="s">
+      <c r="G2" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="H2" s="14" t="s">
+      <c r="H2" s="13" t="s">
         <v>38</v>
       </c>
       <c r="I2" s="7" t="n">
@@ -4640,38 +4624,39 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:M21"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E27" activeCellId="0" sqref="E27"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M21" activeCellId="0" sqref="M21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.67578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="29.44"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="2" style="1" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="32.35"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="2" style="1" width="12.67"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="9" min="8" style="3" width="12.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="29" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="G1" s="24" t="s">
         <v>31</v>
       </c>
       <c r="H1" s="27" t="s">
@@ -4691,7 +4676,7 @@
       <c r="D2" s="7" t="n">
         <v>150</v>
       </c>
-      <c r="E2" s="14" t="n">
+      <c r="E2" s="13" t="n">
         <f aca="false">misc!A2+1</f>
         <v>45656</v>
       </c>
@@ -4709,6 +4694,9 @@
         <f aca="false">AND(ISNUMBER(F2), E2&lt;=F2, F2&lt;=misc!D2)</f>
         <v>1</v>
       </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M21" s="3"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -4732,32 +4720,33 @@
       <selection pane="topLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.67578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="29.44"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="2" style="1" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="32.35"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="2" style="1" width="12.67"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="8" style="3" width="12.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="29" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="G1" s="24" t="s">
         <v>43</v>
       </c>
     </row>
@@ -4771,7 +4760,7 @@
       <c r="D2" s="7" t="n">
         <v>150</v>
       </c>
-      <c r="E2" s="14" t="s">
+      <c r="E2" s="13" t="s">
         <v>44</v>
       </c>
       <c r="F2" s="7" t="n">
@@ -4803,32 +4792,33 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.67578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="37.7"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="2" style="1" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="41.44"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="2" style="1" width="12.67"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="8" style="3" width="12.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="29" t="s">
         <v>45</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="24" t="s">
         <v>46</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="G1" s="24" t="s">
         <v>47</v>
       </c>
     </row>
@@ -4842,7 +4832,7 @@
       <c r="D2" s="7" t="n">
         <v>150</v>
       </c>
-      <c r="E2" s="14" t="s">
+      <c r="E2" s="13" t="s">
         <v>48</v>
       </c>
       <c r="F2" s="7" t="s">
@@ -4874,43 +4864,44 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.67578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="37.7"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="8" min="2" style="1" width="11.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="21.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="13.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="41.44"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="8" min="2" style="1" width="12.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="15.28"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="11" style="3" width="12.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="29" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="24" t="s">
         <v>52</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="G1" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="H1" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="I1" s="10" t="s">
+      <c r="I1" s="24" t="s">
         <v>55</v>
       </c>
-      <c r="J1" s="10" t="s">
+      <c r="J1" s="24" t="s">
         <v>56</v>
       </c>
     </row>
@@ -4924,10 +4915,10 @@
       <c r="D2" s="7" t="n">
         <v>150</v>
       </c>
-      <c r="E2" s="14" t="s">
+      <c r="E2" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="F2" s="13" t="s">
         <v>35</v>
       </c>
       <c r="G2" s="7" t="n">
@@ -4965,11 +4956,12 @@
       <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.71484375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.57"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="2" style="7" width="11.57"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="5" style="6" width="11.57"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12.71"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="2" style="7" width="12.71"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="5" style="6" width="12.71"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="7" style="3" width="12.71"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5061,8 +5053,8 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="13"/>
-      <c r="C5" s="13"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="12"/>
@@ -5105,204 +5097,204 @@
       <c r="C15" s="12"/>
     </row>
     <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="14"/>
-      <c r="C16" s="14"/>
+      <c r="B16" s="13"/>
+      <c r="C16" s="13"/>
     </row>
     <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="14"/>
-      <c r="C17" s="14"/>
+      <c r="B17" s="13"/>
+      <c r="C17" s="13"/>
     </row>
     <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="14"/>
-      <c r="C18" s="14"/>
+      <c r="B18" s="13"/>
+      <c r="C18" s="13"/>
     </row>
     <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="14"/>
-      <c r="C19" s="14"/>
+      <c r="B19" s="13"/>
+      <c r="C19" s="13"/>
     </row>
     <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="14"/>
-      <c r="C20" s="14"/>
+      <c r="B20" s="13"/>
+      <c r="C20" s="13"/>
     </row>
     <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="14"/>
-      <c r="C21" s="14"/>
+      <c r="B21" s="13"/>
+      <c r="C21" s="13"/>
     </row>
     <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="14"/>
-      <c r="C22" s="14"/>
+      <c r="B22" s="13"/>
+      <c r="C22" s="13"/>
     </row>
     <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="14"/>
-      <c r="C23" s="14"/>
+      <c r="B23" s="13"/>
+      <c r="C23" s="13"/>
     </row>
     <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="14"/>
-      <c r="C24" s="14"/>
+      <c r="B24" s="13"/>
+      <c r="C24" s="13"/>
     </row>
     <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="14"/>
-      <c r="C25" s="14"/>
+      <c r="B25" s="13"/>
+      <c r="C25" s="13"/>
     </row>
     <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="14"/>
-      <c r="C26" s="14"/>
+      <c r="B26" s="13"/>
+      <c r="C26" s="13"/>
     </row>
     <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="14"/>
-      <c r="C27" s="14"/>
+      <c r="B27" s="13"/>
+      <c r="C27" s="13"/>
     </row>
     <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="14"/>
-      <c r="C28" s="14"/>
+      <c r="B28" s="13"/>
+      <c r="C28" s="13"/>
     </row>
     <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="14"/>
-      <c r="C29" s="14"/>
+      <c r="B29" s="13"/>
+      <c r="C29" s="13"/>
     </row>
     <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="14"/>
-      <c r="C30" s="14"/>
+      <c r="B30" s="13"/>
+      <c r="C30" s="13"/>
     </row>
     <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="14"/>
-      <c r="C31" s="14"/>
+      <c r="B31" s="13"/>
+      <c r="C31" s="13"/>
     </row>
     <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B32" s="14"/>
-      <c r="C32" s="14"/>
+      <c r="B32" s="13"/>
+      <c r="C32" s="13"/>
     </row>
     <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B33" s="14"/>
-      <c r="C33" s="14"/>
+      <c r="B33" s="13"/>
+      <c r="C33" s="13"/>
     </row>
     <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B34" s="14"/>
-      <c r="C34" s="14"/>
+      <c r="B34" s="13"/>
+      <c r="C34" s="13"/>
     </row>
     <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B35" s="14"/>
-      <c r="C35" s="14"/>
+      <c r="B35" s="13"/>
+      <c r="C35" s="13"/>
     </row>
     <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B36" s="14"/>
-      <c r="C36" s="14"/>
+      <c r="B36" s="13"/>
+      <c r="C36" s="13"/>
     </row>
     <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B37" s="14"/>
-      <c r="C37" s="14"/>
+      <c r="B37" s="13"/>
+      <c r="C37" s="13"/>
     </row>
     <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B38" s="14"/>
-      <c r="C38" s="14"/>
+      <c r="B38" s="13"/>
+      <c r="C38" s="13"/>
     </row>
     <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B39" s="14"/>
-      <c r="C39" s="14"/>
+      <c r="B39" s="13"/>
+      <c r="C39" s="13"/>
     </row>
     <row r="40" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B40" s="14"/>
-      <c r="C40" s="14"/>
+      <c r="B40" s="13"/>
+      <c r="C40" s="13"/>
     </row>
     <row r="41" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B41" s="14"/>
-      <c r="C41" s="14"/>
+      <c r="B41" s="13"/>
+      <c r="C41" s="13"/>
     </row>
     <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B42" s="14"/>
-      <c r="C42" s="14"/>
+      <c r="B42" s="13"/>
+      <c r="C42" s="13"/>
     </row>
     <row r="43" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B43" s="14"/>
-      <c r="C43" s="14"/>
+      <c r="B43" s="13"/>
+      <c r="C43" s="13"/>
     </row>
     <row r="44" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B44" s="14"/>
-      <c r="C44" s="14"/>
+      <c r="B44" s="13"/>
+      <c r="C44" s="13"/>
     </row>
     <row r="45" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B45" s="14"/>
-      <c r="C45" s="14"/>
+      <c r="B45" s="13"/>
+      <c r="C45" s="13"/>
     </row>
     <row r="46" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B46" s="14"/>
-      <c r="C46" s="14"/>
+      <c r="B46" s="13"/>
+      <c r="C46" s="13"/>
     </row>
     <row r="47" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B47" s="14"/>
-      <c r="C47" s="14"/>
+      <c r="B47" s="13"/>
+      <c r="C47" s="13"/>
     </row>
     <row r="48" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B48" s="14"/>
-      <c r="C48" s="14"/>
+      <c r="B48" s="13"/>
+      <c r="C48" s="13"/>
     </row>
     <row r="49" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B49" s="14"/>
-      <c r="C49" s="14"/>
+      <c r="B49" s="13"/>
+      <c r="C49" s="13"/>
     </row>
     <row r="50" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B50" s="14"/>
-      <c r="C50" s="14"/>
+      <c r="B50" s="13"/>
+      <c r="C50" s="13"/>
     </row>
     <row r="51" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B51" s="14"/>
-      <c r="C51" s="14"/>
+      <c r="B51" s="13"/>
+      <c r="C51" s="13"/>
     </row>
     <row r="52" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B52" s="14"/>
-      <c r="C52" s="14"/>
+      <c r="B52" s="13"/>
+      <c r="C52" s="13"/>
     </row>
     <row r="53" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B53" s="14"/>
-      <c r="C53" s="14"/>
+      <c r="B53" s="13"/>
+      <c r="C53" s="13"/>
     </row>
     <row r="54" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B54" s="14"/>
-      <c r="C54" s="14"/>
+      <c r="B54" s="13"/>
+      <c r="C54" s="13"/>
     </row>
     <row r="55" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B55" s="14"/>
-      <c r="C55" s="14"/>
+      <c r="B55" s="13"/>
+      <c r="C55" s="13"/>
     </row>
     <row r="56" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B56" s="14"/>
-      <c r="C56" s="14"/>
+      <c r="B56" s="13"/>
+      <c r="C56" s="13"/>
     </row>
     <row r="57" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B57" s="14"/>
-      <c r="C57" s="14"/>
+      <c r="B57" s="13"/>
+      <c r="C57" s="13"/>
     </row>
     <row r="58" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B58" s="14"/>
-      <c r="C58" s="14"/>
+      <c r="B58" s="13"/>
+      <c r="C58" s="13"/>
     </row>
     <row r="59" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B59" s="14"/>
-      <c r="C59" s="14"/>
+      <c r="B59" s="13"/>
+      <c r="C59" s="13"/>
     </row>
     <row r="60" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B60" s="14"/>
-      <c r="C60" s="14"/>
+      <c r="B60" s="13"/>
+      <c r="C60" s="13"/>
     </row>
     <row r="61" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B61" s="14"/>
-      <c r="C61" s="14"/>
+      <c r="B61" s="13"/>
+      <c r="C61" s="13"/>
     </row>
     <row r="62" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B62" s="14"/>
-      <c r="C62" s="14"/>
+      <c r="B62" s="13"/>
+      <c r="C62" s="13"/>
     </row>
     <row r="63" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B63" s="14"/>
-      <c r="C63" s="14"/>
+      <c r="B63" s="13"/>
+      <c r="C63" s="13"/>
     </row>
     <row r="64" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B64" s="14"/>
-      <c r="C64" s="14"/>
+      <c r="B64" s="13"/>
+      <c r="C64" s="13"/>
     </row>
     <row r="65" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B65" s="14"/>
-      <c r="C65" s="14"/>
+      <c r="B65" s="13"/>
+      <c r="C65" s="13"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -5321,32 +5313,33 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G1048576"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.71484375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="22.71"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.57"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="3" style="6" width="11.57"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="4" style="15" width="11.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="24.96"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="12.71"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="3" style="6" width="12.71"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="12.71"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="5" style="3" width="12.71"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="5" t="b">
+      <c r="C1" s="16" t="b">
         <f aca="false">AND(C2:C938)</f>
         <v>1</v>
       </c>
-      <c r="D1" s="5" t="b">
+      <c r="D1" s="16" t="b">
         <f aca="false">AND(D2:D938)</f>
         <v>1</v>
       </c>
@@ -5354,7 +5347,7 @@
       <c r="G1" s="1"/>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -5445,165 +5438,6 @@
       <c r="C15" s="17"/>
       <c r="D15" s="17"/>
     </row>
-    <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="3"/>
-      <c r="B16" s="3"/>
-    </row>
-    <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="3"/>
-      <c r="B17" s="3"/>
-    </row>
-    <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="3"/>
-      <c r="B18" s="3"/>
-    </row>
-    <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="3"/>
-      <c r="B19" s="3"/>
-    </row>
-    <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="3"/>
-      <c r="B20" s="3"/>
-    </row>
-    <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="3"/>
-      <c r="B21" s="3"/>
-    </row>
-    <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="3"/>
-      <c r="B22" s="3"/>
-    </row>
-    <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="3"/>
-      <c r="B23" s="3"/>
-    </row>
-    <row r="1048450" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048451" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048452" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048453" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048454" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048455" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048456" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048457" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048458" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048459" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048460" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048461" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048462" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048463" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048464" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048465" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048466" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048467" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048468" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048469" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048470" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048471" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048472" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048473" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048474" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048475" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048476" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048477" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048478" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048479" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048480" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048481" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048482" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048483" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048484" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048485" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048486" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048487" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048488" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048489" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048490" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048491" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048492" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048493" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048494" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048495" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048496" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048497" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048498" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048499" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048500" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048501" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048502" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048503" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048504" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048505" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048506" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048507" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048508" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048509" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048510" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048511" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048512" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048513" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048514" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048515" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048516" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048517" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048518" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048519" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048520" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048521" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048522" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048523" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048524" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048525" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048526" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048527" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048528" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048529" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048530" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048531" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048532" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048533" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048534" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048535" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048536" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048537" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048538" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048539" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048540" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048541" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048542" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048543" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048544" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048545" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048546" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048547" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048548" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048549" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048550" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048551" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048552" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048553" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048554" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048555" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048556" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048557" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048558" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048559" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048560" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048561" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048562" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048563" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048564" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048565" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048566" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048567" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -5627,149 +5461,150 @@
       <selection pane="topLeft" activeCell="G18" activeCellId="0" sqref="G18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.71484375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="22.71"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.57"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="3" style="7" width="11.57"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="8" min="7" style="18" width="11.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="24.96"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="12.71"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="3" style="7" width="12.71"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="8" min="7" style="6" width="12.71"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="9" style="3" width="12.71"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="5" t="e">
+      <c r="G1" s="16" t="e">
         <f aca="false">AND(G2:G938)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="H1" s="5" t="e">
+      <c r="H1" s="16" t="e">
         <f aca="false">AND(H2:H938)</f>
         <v>#VALUE!</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="17"/>
       <c r="H2" s="17"/>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="17"/>
       <c r="H3" s="17"/>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C4" s="19"/>
-      <c r="D4" s="19"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="17"/>
       <c r="H4" s="17"/>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C5" s="19"/>
-      <c r="D5" s="19"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="17"/>
       <c r="H5" s="17"/>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C6" s="19"/>
-      <c r="D6" s="19"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="12"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="17"/>
       <c r="H6" s="17"/>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C7" s="19"/>
-      <c r="D7" s="19"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="12"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="17"/>
       <c r="H7" s="17"/>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C8" s="19"/>
-      <c r="D8" s="19"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="12"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="17"/>
       <c r="H8" s="17"/>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C9" s="19"/>
-      <c r="D9" s="19"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="12"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="17"/>
       <c r="H9" s="17"/>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C10" s="19"/>
-      <c r="D10" s="19"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="17"/>
       <c r="H10" s="17"/>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C11" s="19"/>
-      <c r="D11" s="19"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="12"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
       <c r="G11" s="17"/>
       <c r="H11" s="17"/>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C12" s="19"/>
-      <c r="D12" s="19"/>
+      <c r="C12" s="12"/>
+      <c r="D12" s="12"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
       <c r="G12" s="17"/>
       <c r="H12" s="17"/>
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C13" s="19"/>
-      <c r="D13" s="19"/>
+      <c r="C13" s="12"/>
+      <c r="D13" s="12"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
       <c r="G13" s="17"/>
       <c r="H13" s="17"/>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C14" s="19"/>
-      <c r="D14" s="19"/>
+      <c r="C14" s="12"/>
+      <c r="D14" s="12"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
       <c r="G14" s="17"/>
       <c r="H14" s="17"/>
     </row>
     <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C15" s="19"/>
-      <c r="D15" s="19"/>
+      <c r="C15" s="12"/>
+      <c r="D15" s="12"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
       <c r="G15" s="17"/>
@@ -6125,34 +5960,35 @@
   <dimension ref="A1:F70"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+      <selection pane="topLeft" activeCell="J6" activeCellId="0" sqref="J6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.71484375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="22.71"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.57"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="3" style="7" width="11.57"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="11.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="24.96"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="12.71"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="3" style="7" width="12.71"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="12.71"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="7" style="3" width="12.71"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="18" t="s">
         <v>15</v>
       </c>
     </row>
@@ -6523,32 +6359,33 @@
       <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.71484375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="14.21"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="2" style="7" width="11.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="15.62"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="2" style="7" width="12.71"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="6" style="3" width="12.71"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="18" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="14"/>
-      <c r="C2" s="20"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="19"/>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="12"/>
@@ -6980,31 +6817,32 @@
       <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.71484375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="22.71"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.57"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="3" style="7" width="11.57"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="11.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="24.96"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="12.71"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="3" style="7" width="12.71"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="12.71"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="7" style="3" width="12.71"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="18" t="s">
         <v>15</v>
       </c>
     </row>
@@ -7375,180 +7213,181 @@
       <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.71484375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.57"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="2" style="7" width="11.57"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12.71"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="2" style="7" width="12.71"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="6" style="3" width="12.71"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="18" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="14"/>
-      <c r="C2" s="20"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="19"/>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="14"/>
-      <c r="C3" s="14"/>
+      <c r="B3" s="13"/>
+      <c r="C3" s="13"/>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="14"/>
-      <c r="C4" s="14"/>
+      <c r="B4" s="13"/>
+      <c r="C4" s="13"/>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="14"/>
-      <c r="C5" s="14"/>
+      <c r="B5" s="13"/>
+      <c r="C5" s="13"/>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="14"/>
-      <c r="C6" s="14"/>
+      <c r="B6" s="13"/>
+      <c r="C6" s="13"/>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="14"/>
-      <c r="C7" s="14"/>
+      <c r="B7" s="13"/>
+      <c r="C7" s="13"/>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="14"/>
-      <c r="C8" s="14"/>
+      <c r="B8" s="13"/>
+      <c r="C8" s="13"/>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="14"/>
-      <c r="C9" s="14"/>
+      <c r="B9" s="13"/>
+      <c r="C9" s="13"/>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="14"/>
-      <c r="C10" s="14"/>
+      <c r="B10" s="13"/>
+      <c r="C10" s="13"/>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="14"/>
-      <c r="C11" s="14"/>
+      <c r="B11" s="13"/>
+      <c r="C11" s="13"/>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="14"/>
-      <c r="C12" s="14"/>
+      <c r="B12" s="13"/>
+      <c r="C12" s="13"/>
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="14"/>
-      <c r="C13" s="14"/>
+      <c r="B13" s="13"/>
+      <c r="C13" s="13"/>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="14"/>
-      <c r="C14" s="14"/>
+      <c r="B14" s="13"/>
+      <c r="C14" s="13"/>
     </row>
     <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="14"/>
-      <c r="C15" s="14"/>
+      <c r="B15" s="13"/>
+      <c r="C15" s="13"/>
     </row>
     <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="14"/>
-      <c r="C16" s="14"/>
+      <c r="B16" s="13"/>
+      <c r="C16" s="13"/>
     </row>
     <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="14"/>
-      <c r="C17" s="14"/>
+      <c r="B17" s="13"/>
+      <c r="C17" s="13"/>
     </row>
     <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="14"/>
-      <c r="C18" s="14"/>
+      <c r="B18" s="13"/>
+      <c r="C18" s="13"/>
     </row>
     <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="14"/>
-      <c r="C19" s="14"/>
+      <c r="B19" s="13"/>
+      <c r="C19" s="13"/>
     </row>
     <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="14"/>
-      <c r="C20" s="14"/>
+      <c r="B20" s="13"/>
+      <c r="C20" s="13"/>
     </row>
     <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="14"/>
-      <c r="C21" s="14"/>
+      <c r="B21" s="13"/>
+      <c r="C21" s="13"/>
     </row>
     <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="14"/>
-      <c r="C22" s="14"/>
+      <c r="B22" s="13"/>
+      <c r="C22" s="13"/>
     </row>
     <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="14"/>
-      <c r="C23" s="14"/>
+      <c r="B23" s="13"/>
+      <c r="C23" s="13"/>
     </row>
     <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="14"/>
-      <c r="C24" s="14"/>
+      <c r="B24" s="13"/>
+      <c r="C24" s="13"/>
     </row>
     <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="14"/>
-      <c r="C25" s="14"/>
+      <c r="B25" s="13"/>
+      <c r="C25" s="13"/>
     </row>
     <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="14"/>
-      <c r="C26" s="14"/>
+      <c r="B26" s="13"/>
+      <c r="C26" s="13"/>
     </row>
     <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="14"/>
-      <c r="C27" s="14"/>
+      <c r="B27" s="13"/>
+      <c r="C27" s="13"/>
     </row>
     <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="14"/>
-      <c r="C28" s="14"/>
+      <c r="B28" s="13"/>
+      <c r="C28" s="13"/>
     </row>
     <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="14"/>
-      <c r="C29" s="14"/>
+      <c r="B29" s="13"/>
+      <c r="C29" s="13"/>
     </row>
     <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="14"/>
-      <c r="C30" s="14"/>
+      <c r="B30" s="13"/>
+      <c r="C30" s="13"/>
     </row>
     <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="14"/>
-      <c r="C31" s="14"/>
+      <c r="B31" s="13"/>
+      <c r="C31" s="13"/>
     </row>
     <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B32" s="14"/>
-      <c r="C32" s="14"/>
+      <c r="B32" s="13"/>
+      <c r="C32" s="13"/>
     </row>
     <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B33" s="14"/>
-      <c r="C33" s="14"/>
+      <c r="B33" s="13"/>
+      <c r="C33" s="13"/>
     </row>
     <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B34" s="14"/>
-      <c r="C34" s="14"/>
+      <c r="B34" s="13"/>
+      <c r="C34" s="13"/>
     </row>
     <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B35" s="14"/>
-      <c r="C35" s="14"/>
+      <c r="B35" s="13"/>
+      <c r="C35" s="13"/>
     </row>
     <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B36" s="14"/>
-      <c r="C36" s="14"/>
+      <c r="B36" s="13"/>
+      <c r="C36" s="13"/>
     </row>
     <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B37" s="14"/>
-      <c r="C37" s="14"/>
+      <c r="B37" s="13"/>
+      <c r="C37" s="13"/>
     </row>
     <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B38" s="14"/>
-      <c r="C38" s="14"/>
+      <c r="B38" s="13"/>
+      <c r="C38" s="13"/>
     </row>
     <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B39" s="14"/>
-      <c r="C39" s="14"/>
+      <c r="B39" s="13"/>
+      <c r="C39" s="13"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -7572,36 +7411,37 @@
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.71484375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="21.14"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="2" style="7" width="11.57"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="4" style="6" width="11.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="23.24"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="2" style="7" width="12.71"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="4" style="6" width="12.71"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="5" style="3" width="12.71"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="5" t="b">
+      <c r="D1" s="16" t="b">
         <f aca="false">AND(D2:D900)</f>
         <v>1</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="22" t="n">
+      <c r="B2" s="21" t="n">
         <v>45637</v>
       </c>
-      <c r="C2" s="22" t="n">
+      <c r="C2" s="21" t="n">
         <v>45672</v>
       </c>
       <c r="D2" s="6" t="b">
@@ -7610,13 +7450,13 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="21" t="s">
+      <c r="A3" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="22" t="n">
+      <c r="B3" s="21" t="n">
         <v>45673</v>
       </c>
-      <c r="C3" s="22" t="n">
+      <c r="C3" s="21" t="n">
         <v>45701</v>
       </c>
       <c r="D3" s="6" t="b">
@@ -7625,194 +7465,194 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="23"/>
-      <c r="B4" s="20"/>
-      <c r="C4" s="20"/>
+      <c r="A4" s="22"/>
+      <c r="B4" s="19"/>
+      <c r="C4" s="19"/>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="23"/>
-      <c r="B5" s="20"/>
-      <c r="C5" s="20"/>
+      <c r="A5" s="22"/>
+      <c r="B5" s="19"/>
+      <c r="C5" s="19"/>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="23"/>
-      <c r="B6" s="20"/>
-      <c r="C6" s="20"/>
+      <c r="A6" s="22"/>
+      <c r="B6" s="19"/>
+      <c r="C6" s="19"/>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="23"/>
-      <c r="B7" s="20"/>
-      <c r="C7" s="20"/>
+      <c r="A7" s="22"/>
+      <c r="B7" s="19"/>
+      <c r="C7" s="19"/>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="23"/>
-      <c r="B8" s="14"/>
-      <c r="C8" s="20"/>
+      <c r="A8" s="22"/>
+      <c r="B8" s="13"/>
+      <c r="C8" s="19"/>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="23"/>
-      <c r="B9" s="20"/>
-      <c r="C9" s="20"/>
+      <c r="A9" s="22"/>
+      <c r="B9" s="19"/>
+      <c r="C9" s="19"/>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="23"/>
-      <c r="B10" s="14"/>
-      <c r="C10" s="14"/>
+      <c r="A10" s="22"/>
+      <c r="B10" s="13"/>
+      <c r="C10" s="13"/>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="23"/>
-      <c r="B11" s="14"/>
-      <c r="C11" s="14"/>
+      <c r="A11" s="22"/>
+      <c r="B11" s="13"/>
+      <c r="C11" s="13"/>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="23"/>
-      <c r="B12" s="14"/>
-      <c r="C12" s="14"/>
+      <c r="A12" s="22"/>
+      <c r="B12" s="13"/>
+      <c r="C12" s="13"/>
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="23"/>
-      <c r="B13" s="14"/>
-      <c r="C13" s="14"/>
+      <c r="A13" s="22"/>
+      <c r="B13" s="13"/>
+      <c r="C13" s="13"/>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="14"/>
-      <c r="C14" s="14"/>
+      <c r="B14" s="13"/>
+      <c r="C14" s="13"/>
     </row>
     <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="14"/>
-      <c r="C15" s="14"/>
+      <c r="B15" s="13"/>
+      <c r="C15" s="13"/>
     </row>
     <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="14"/>
-      <c r="C16" s="14"/>
+      <c r="B16" s="13"/>
+      <c r="C16" s="13"/>
     </row>
     <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="14"/>
-      <c r="C17" s="14"/>
+      <c r="B17" s="13"/>
+      <c r="C17" s="13"/>
     </row>
     <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="14"/>
-      <c r="C18" s="14"/>
+      <c r="B18" s="13"/>
+      <c r="C18" s="13"/>
     </row>
     <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="14"/>
-      <c r="C19" s="14"/>
+      <c r="B19" s="13"/>
+      <c r="C19" s="13"/>
     </row>
     <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="14"/>
-      <c r="C20" s="14"/>
+      <c r="B20" s="13"/>
+      <c r="C20" s="13"/>
     </row>
     <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="14"/>
-      <c r="C21" s="14"/>
+      <c r="B21" s="13"/>
+      <c r="C21" s="13"/>
     </row>
     <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="14"/>
-      <c r="C22" s="14"/>
+      <c r="B22" s="13"/>
+      <c r="C22" s="13"/>
     </row>
     <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="14"/>
-      <c r="C23" s="14"/>
+      <c r="B23" s="13"/>
+      <c r="C23" s="13"/>
     </row>
     <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="14"/>
-      <c r="C24" s="14"/>
+      <c r="B24" s="13"/>
+      <c r="C24" s="13"/>
     </row>
     <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="14"/>
-      <c r="C25" s="14"/>
+      <c r="B25" s="13"/>
+      <c r="C25" s="13"/>
     </row>
     <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="14"/>
-      <c r="C26" s="14"/>
+      <c r="B26" s="13"/>
+      <c r="C26" s="13"/>
     </row>
     <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="14"/>
-      <c r="C27" s="14"/>
+      <c r="B27" s="13"/>
+      <c r="C27" s="13"/>
     </row>
     <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="14"/>
-      <c r="C28" s="14"/>
+      <c r="B28" s="13"/>
+      <c r="C28" s="13"/>
     </row>
     <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="14"/>
-      <c r="C29" s="14"/>
+      <c r="B29" s="13"/>
+      <c r="C29" s="13"/>
     </row>
     <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="14"/>
-      <c r="C30" s="14"/>
+      <c r="B30" s="13"/>
+      <c r="C30" s="13"/>
     </row>
     <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="14"/>
-      <c r="C31" s="14"/>
+      <c r="B31" s="13"/>
+      <c r="C31" s="13"/>
     </row>
     <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B32" s="14"/>
-      <c r="C32" s="14"/>
+      <c r="B32" s="13"/>
+      <c r="C32" s="13"/>
     </row>
     <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B33" s="14"/>
-      <c r="C33" s="14"/>
+      <c r="B33" s="13"/>
+      <c r="C33" s="13"/>
     </row>
     <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B34" s="14"/>
-      <c r="C34" s="14"/>
+      <c r="B34" s="13"/>
+      <c r="C34" s="13"/>
     </row>
     <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B35" s="14"/>
-      <c r="C35" s="14"/>
+      <c r="B35" s="13"/>
+      <c r="C35" s="13"/>
     </row>
     <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B36" s="14"/>
-      <c r="C36" s="14"/>
+      <c r="B36" s="13"/>
+      <c r="C36" s="13"/>
     </row>
     <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B37" s="14"/>
-      <c r="C37" s="14"/>
+      <c r="B37" s="13"/>
+      <c r="C37" s="13"/>
     </row>
     <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B38" s="14"/>
-      <c r="C38" s="14"/>
+      <c r="B38" s="13"/>
+      <c r="C38" s="13"/>
     </row>
     <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B39" s="14"/>
-      <c r="C39" s="14"/>
+      <c r="B39" s="13"/>
+      <c r="C39" s="13"/>
     </row>
     <row r="40" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B40" s="14"/>
-      <c r="C40" s="14"/>
+      <c r="B40" s="13"/>
+      <c r="C40" s="13"/>
     </row>
     <row r="41" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B41" s="14"/>
-      <c r="C41" s="14"/>
+      <c r="B41" s="13"/>
+      <c r="C41" s="13"/>
     </row>
     <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B42" s="14"/>
-      <c r="C42" s="14"/>
+      <c r="B42" s="13"/>
+      <c r="C42" s="13"/>
     </row>
     <row r="43" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B43" s="14"/>
-      <c r="C43" s="14"/>
+      <c r="B43" s="13"/>
+      <c r="C43" s="13"/>
     </row>
     <row r="44" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B44" s="14"/>
-      <c r="C44" s="14"/>
+      <c r="B44" s="13"/>
+      <c r="C44" s="13"/>
     </row>
     <row r="45" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B45" s="14"/>
-      <c r="C45" s="14"/>
+      <c r="B45" s="13"/>
+      <c r="C45" s="13"/>
     </row>
     <row r="46" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B46" s="14"/>
-      <c r="C46" s="14"/>
+      <c r="B46" s="13"/>
+      <c r="C46" s="13"/>
     </row>
     <row r="47" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B47" s="14"/>
-      <c r="C47" s="14"/>
+      <c r="B47" s="13"/>
+      <c r="C47" s="13"/>
     </row>
     <row r="48" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B48" s="14"/>
-      <c r="C48" s="14"/>
+      <c r="B48" s="13"/>
+      <c r="C48" s="13"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>